<commit_message>
changes in data file, prepared ml_tutorial
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -125,6 +125,96 @@
   </si>
   <si>
     <t xml:space="preserve">Como se llama el presidente del gobierno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U mnie to nie zadziałało.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czy moge prosić o jakąś podpowiedź?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teraz możesz zobaczyć się ze swoim lekarzem bez wychodzenia z domu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codziennie po lekcjach gram w tenisa ze swoim najlepszym kolegą.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prawdziwych przyjaciół poznajemy w biedzie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dzien dobry, proszę o informację, jak otworzyć plik na dysku.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Każdego dnia ćwiczę przez pół godziny rano i wieczorem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kierowca autobusu nosi zielone okulary przeciwsłoneczne.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O ogrodzie zoologicznym można spotkać mnóstwo zwierząt egzotycznych.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mamo, nudzi mi się, co mogę zrobić?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have lots of free on-line games, songs, stories and activities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a free app, very useful for your kids.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you running out of ideas on how to teach your children?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This core is theoretically enough for everyday life.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At this level students could start to move on their own.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When will a coronavirus vaccine be ready and how would it work?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social distancing likely to go on long after the lockdown.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He thinks american music is great and the people around here are friendly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get a one month free trial.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Older generation must give more to the young.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justicia prepara una ley exprés para evitar el colapso en los tribunales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se producen frutas cada vez con más azúcar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las ballenas del Atlántico tienen altos niveles de químicos procedentes del plástico.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No ejecutar en páginas de este sitio web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barcelona es una ciudad española, capital de la comunidad autónoma de Cataluña.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La ciudad posee un clima mediterráneo con influencias marítimas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cada distrito funciona como un ente político con competencias propias.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¡Bienvenido a la única web especializada en actividades y excursiones en el Parque Nacional del Teide!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atendiendo a las clases existen dos tipos de desempleo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A los efectos de la base reguladora no se incluirá en la misma las horas extraordinarias.</t>
   </si>
 </sst>
 </file>
@@ -232,15 +322,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F59" activeCellId="0" sqref="F59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="85.07"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,6 +578,246 @@
         <v>34</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" s="0" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change the format of file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -325,10 +325,10 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F59" activeCellId="0" sqref="F59"/>
+      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="85.07"/>
   </cols>

</xml_diff>

<commit_message>
added file with french data, corrections in previous files
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">I would like to be an astronaut.</t>
   </si>
   <si>
-    <t xml:space="preserve">Please, send mi an envelope full of paper.</t>
+    <t xml:space="preserve">Please, send me an envelope full of paper.</t>
   </si>
   <si>
     <t xml:space="preserve">We will spend most of the meeting sharing and discussing this information.</t>
@@ -325,10 +325,10 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="85.07"/>
   </cols>

</xml_diff>